<commit_message>
feat: add single and multi corrector
</commit_message>
<xml_diff>
--- a/output/inference_results/test_sheets/batch_001/test_sheet (1).xlsx
+++ b/output/inference_results/test_sheets/batch_001/test_sheet (1).xlsx
@@ -451,22 +451,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>钾离子（K）</t>
+          <t>钾离子</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>钾离子（K）</t>
+          <t>K</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>4.20</t>
+          <t>4.2</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>mmo1/L</t>
+          <t>mmol/L</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -478,14 +478,10 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2 钠离子（Na）</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2 钠离子（Na）</t>
-        </is>
-      </c>
+          <t>钠离子</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
           <t>140</t>
@@ -493,7 +489,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>mmo1/L</t>
+          <t>mmol/L</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -505,12 +501,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>氯离子（Cl）</t>
+          <t>氯离子</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>氯离子（Cl）</t>
+          <t>Cl</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -520,7 +516,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>mmo1/L</t>
+          <t>mmol/L</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -532,14 +528,10 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>4总二氧化碳（TCO2）</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>4总二氧化碳（TCO2）</t>
-        </is>
-      </c>
+          <t>总二氧化碳</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
           <t>29.4</t>
@@ -559,14 +551,10 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>5尿素（UREA）</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>5尿素（UREA）</t>
-        </is>
-      </c>
+          <t>尿素</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
           <t>7.9</t>
@@ -586,14 +574,10 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>6肌酐（CR）</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>6肌酐（CR）</t>
-        </is>
-      </c>
+          <t>肌酐</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
           <t>105</t>
@@ -613,14 +597,10 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>7尿酸（UA）</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>7尿酸（UA）</t>
-        </is>
-      </c>
+          <t>尿酸</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr">
         <is>
           <t>298</t>
@@ -628,7 +608,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>umol/L</t>
+          <t>μmol/L</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -640,14 +620,10 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>8 丙氨酸氨基转移酶（ALT）</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>8 丙氨酸氨基转移酶（ALT）</t>
-        </is>
-      </c>
+          <t>丙氨酸氨基转移酶</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
           <t>65</t>
@@ -667,14 +643,10 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>9 天门冬氨酸氨基转移酶（AST）</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>9 天门冬氨酸氨基转移酶（AST）</t>
-        </is>
-      </c>
+          <t>天门冬氨酸氨基转移酶</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr">
         <is>
           <t>20</t>
@@ -694,14 +666,10 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>10转氨酶比值（AST/ALT）</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>10转氨酶比值（AST/ALT）</t>
-        </is>
-      </c>
+          <t>转氨酶比值</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr">
         <is>
           <t>0.3</t>
@@ -717,14 +685,10 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>11总蛋白（TP）</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>11总蛋白（TP）</t>
-        </is>
-      </c>
+          <t>总蛋白</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr">
         <is>
           <t>67.8</t>
@@ -744,14 +708,10 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>12白蛋白（ALB）</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>12白蛋白（ALB）</t>
-        </is>
-      </c>
+          <t>白蛋白</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr">
         <is>
           <t>43.0</t>
@@ -771,14 +731,10 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>13球蛋白（G）</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>13球蛋白（G）</t>
-        </is>
-      </c>
+          <t>球蛋白</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr">
         <is>
           <t>24.8</t>
@@ -798,14 +754,10 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>14白/球比值（A/G</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>14白/球比值（A/G</t>
-        </is>
-      </c>
+          <t>白/球比值</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr">
         <is>
           <t>1.7</t>
@@ -821,14 +773,10 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>15总胆红素（TBIL）</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>15总胆红素（TBIL）</t>
-        </is>
-      </c>
+          <t>总胆红素</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr">
         <is>
           <t>8.1</t>
@@ -848,14 +796,10 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>16直接胆红素（DBIL）</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>16直接胆红素（DBIL）</t>
-        </is>
-      </c>
+          <t>直接胆红素</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr">
         <is>
           <t>3.0</t>
@@ -863,7 +807,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>umol/L</t>
+          <t>μmol/L</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -875,14 +819,10 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>17间接胆红素（IBIL）</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>17间接胆红素（IBIL）</t>
-        </is>
-      </c>
+          <t>间接胆红素</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr">
         <is>
           <t>5.1</t>
@@ -890,7 +830,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>mo1/L</t>
+          <t>mol/L</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -902,14 +842,10 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>18葡萄糖（GLU）</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>18葡萄糖（GLU）</t>
-        </is>
-      </c>
+          <t>葡萄糖</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr">
         <is>
           <t>5.46</t>
@@ -929,14 +865,10 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>19甘油三酯（TG）</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>19甘油三酯（TG）</t>
-        </is>
-      </c>
+          <t>甘油三酯</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr">
         <is>
           <t>1.07</t>
@@ -956,14 +888,10 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>20甘油三酯（TG）</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>20甘油三酯（TG）</t>
-        </is>
-      </c>
+          <t>甘油三酯</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr">
         <is>
           <t>95</t>
@@ -983,14 +911,10 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>21总胆固醇（CHOL</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>21总胆固醇（CHOL</t>
-        </is>
-      </c>
+          <t>总胆固醇</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr">
         <is>
           <t>6.44</t>
@@ -1010,14 +934,10 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>22总胆固醇（CHOL）</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>22总胆固醇（CHOL）</t>
-        </is>
-      </c>
+          <t>总胆固醇</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr">
         <is>
           <t>249</t>
@@ -1037,14 +957,10 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>23高密度脂蛋白胆固醇（HDL-C）</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>23高密度脂蛋白胆固醇（HDL-C）</t>
-        </is>
-      </c>
+          <t>高密度脂蛋白胆固醇</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr">
         <is>
           <t>1.58</t>
@@ -1052,7 +968,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>mmo1/L</t>
+          <t>mmol/L</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1064,14 +980,10 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>24高密度脂蛋白胆固醇（HDL-C）</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>24高密度脂蛋白胆固醇（HDL-C）</t>
-        </is>
-      </c>
+          <t>高密度脂蛋白胆固醇</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr">
         <is>
           <t>61</t>
@@ -1091,14 +1003,10 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>25低密度脂蛋白胆固醇（LDL-C）</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>25低密度脂蛋白胆固醇（LDL-C）</t>
-        </is>
-      </c>
+          <t>低密度脂蛋白胆固醇</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr">
         <is>
           <t>4.04</t>
@@ -1118,14 +1026,10 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>26低密度脂蛋白胆固醇（LDL-C）</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>26低密度脂蛋白胆固醇（LDL-C）</t>
-        </is>
-      </c>
+          <t>低密度脂蛋白胆固醇</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr">
         <is>
           <t>156</t>
@@ -1145,14 +1049,10 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>27极低密度脂蛋白胆固醇（VLDL-C</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>27极低密度脂蛋白胆固醇（VLDL-C</t>
-        </is>
-      </c>
+          <t>极低密度脂蛋白胆固醇</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr">
         <is>
           <t>0.82</t>
@@ -1172,14 +1072,10 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>28极低密度脂蛋白胆固醇（VLDL-C</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>28极低密度脂蛋白胆固醇（VLDL-C</t>
-        </is>
-      </c>
+          <t>极低密度脂蛋白胆固醇</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr">
         <is>
           <t>32</t>
@@ -1199,14 +1095,10 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>29非高密度脂蛋白胆固醇（nHDLC）</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>29非高密度脂蛋白胆固醇（nHDLC）</t>
-        </is>
-      </c>
+          <t>非高密度脂蛋白胆固醇</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr">
         <is>
           <t>↑4.86</t>
@@ -1226,14 +1118,10 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>30非高密度脂蛋白胆固醇（nHDLC）</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>30非高密度脂蛋白胆固醇（nHDLC）</t>
-        </is>
-      </c>
+          <t>非高密度脂蛋白胆固醇</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr">
         <is>
           <t>188</t>

</xml_diff>

<commit_message>
refactor: wrap table recognizer
</commit_message>
<xml_diff>
--- a/output/inference_results/test_sheets/batch_001/test_sheet (1).xlsx
+++ b/output/inference_results/test_sheets/batch_001/test_sheet (1).xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,6 +447,31 @@
           <t>参考区间</t>
         </is>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>项目</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>英文缩写</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>结果</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>单位</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>参考区间</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -474,6 +499,27 @@
           <t>3.50-5.30</t>
         </is>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>直接胆红素</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>3.0</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>μmol/L</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>0.0-6.8</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -497,6 +543,27 @@
           <t>137-147</t>
         </is>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>间接胆红素</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>5.1</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>mol/L</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>5.1-13.7</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -524,6 +591,27 @@
           <t>99.0-110.0</t>
         </is>
       </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>葡萄糖</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>5.46</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>mmol/L</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>4.10-5.90</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -547,6 +635,27 @@
           <t>21.0-31.0</t>
         </is>
       </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>甘油三酯</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>1.07</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>mmol/L</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>0.00-1.70</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -570,6 +679,27 @@
           <t>2.8-7.2</t>
         </is>
       </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>甘油三酯</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>95</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>mg/dL</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>0-150</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -593,6 +723,27 @@
           <t>53-123</t>
         </is>
       </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>总胆固醇</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>6.44</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>mmol/L</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>0.00-5.17</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -616,6 +767,27 @@
           <t>208-428</t>
         </is>
       </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>总胆固醇</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>249</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>mg/dL</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>0-200</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -639,6 +811,27 @@
           <t>9-50</t>
         </is>
       </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>高密度脂蛋白胆固醇</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>1.58</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>mmol/L</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>1.03-1.55</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -662,6 +855,27 @@
           <t>15-40</t>
         </is>
       </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>高密度脂蛋白胆固醇</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>mg/dL</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>40-60</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -681,6 +895,27 @@
           <t>1.0-1.5</t>
         </is>
       </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>低密度脂蛋白胆固醇</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>4.04</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>mmol/L</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>0.00-3.36</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -704,6 +939,27 @@
           <t>65.0-85.0</t>
         </is>
       </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>低密度脂蛋白胆固醇</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>156</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>mg/dL</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>0-130</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -727,6 +983,27 @@
           <t>40.0-55.0</t>
         </is>
       </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>极低密度脂蛋白胆固醇</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>0.82</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>mmol/L</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>0.30-1.35</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -750,6 +1027,27 @@
           <t>20.0-40.0</t>
         </is>
       </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>极低密度脂蛋白胆固醇</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>mg/dL</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>12-52</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -769,6 +1067,27 @@
           <t>1.2-2.4</t>
         </is>
       </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>非高密度脂蛋白胆固醇</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>↑4.86</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>mmol/L</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>0.00-4.14</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -792,347 +1111,23 @@
           <t>3.4-20.5</t>
         </is>
       </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>直接胆红素</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>3.0</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>μmol/L</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>0.0-6.8</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>间接胆红素</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>5.1</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>mol/L</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>5.1-13.7</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>葡萄糖</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>5.46</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>mmol/L</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>4.10-5.90</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>甘油三酯</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>1.07</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>mmol/L</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>0.00-1.70</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>甘油三酯</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>95</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>非高密度脂蛋白胆固醇</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>188</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
         <is>
           <t>mg/dL</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>0-150</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>总胆固醇</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr"/>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>6.44</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>mmol/L</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>0.00-5.17</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>总胆固醇</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr"/>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>249</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>mg/dL</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>0-200</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>高密度脂蛋白胆固醇</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr"/>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>1.58</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>mmol/L</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>1.03-1.55</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>高密度脂蛋白胆固醇</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr"/>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>61</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>mg/dL</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>40-60</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>低密度脂蛋白胆固醇</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr"/>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>4.04</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>mmol/L</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>0.00-3.36</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>低密度脂蛋白胆固醇</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr"/>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>156</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>mg/dL</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>0-130</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>极低密度脂蛋白胆固醇</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr"/>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>0.82</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>mmol/L</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>0.30-1.35</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>极低密度脂蛋白胆固醇</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr"/>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>mg/dL</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>12-52</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>非高密度脂蛋白胆固醇</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr"/>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>↑4.86</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>mmol/L</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>0.00-4.14</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>非高密度脂蛋白胆固醇</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr"/>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>188</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>mg/dL</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
+      <c r="J16" t="inlineStr">
         <is>
           <t>0-160</t>
         </is>

</xml_diff>